<commit_message>
Update Microcontroller pinout diagrams.xlsx
</commit_message>
<xml_diff>
--- a/Microcontroller pinout diagrams.xlsx
+++ b/Microcontroller pinout diagrams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2ac6356bae23d48/Documents/^NCODE/SmartCAR/GrabCrab_smartcar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{5A3D812F-B50B-485F-A7E0-E98D5B77DB96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2ADAAE15-B36D-4F46-9181-6BA9795AF891}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{5A3D812F-B50B-485F-A7E0-E98D5B77DB96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{76D7ABDD-86A3-4D9E-9023-A47BF418A7A9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{07093BA4-AFBC-41B7-9BBC-A69CB304ADA0}"/>
   </bookViews>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE36539-01AF-4AFE-888C-B5DD988BEFDF}">
   <dimension ref="B6:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>